<commit_message>
New printing of results to files
</commit_message>
<xml_diff>
--- a/NSU_Results/NSU_Results.xlsx
+++ b/NSU_Results/NSU_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="38400" windowHeight="21120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="48">
   <si>
     <t>Welfare_Gain_Pop(bench)</t>
   </si>
@@ -119,6 +119,51 @@
   </si>
   <si>
     <t>Non-Separable Utility: Sigma=4</t>
+  </si>
+  <si>
+    <t>Threshold_Factor=</t>
+  </si>
+  <si>
+    <t>Wealth_Factor=</t>
+  </si>
+  <si>
+    <t>Threshold=</t>
+  </si>
+  <si>
+    <t>Wealth_Tax_Above=</t>
+  </si>
+  <si>
+    <t>Output_Gain(prct)=</t>
+  </si>
+  <si>
+    <t>W/GDP=</t>
+  </si>
+  <si>
+    <t>Wealth_held_by_Top_1%</t>
+  </si>
+  <si>
+    <t>Wealth_held_by_Top_10%</t>
+  </si>
+  <si>
+    <t>GBAR_exp=</t>
+  </si>
+  <si>
+    <t>QBAR_exp=</t>
+  </si>
+  <si>
+    <t>NBAR_exp=</t>
+  </si>
+  <si>
+    <t>YBAR_exp=</t>
+  </si>
+  <si>
+    <t>EBAR_exp=</t>
+  </si>
+  <si>
+    <t>rr_exp=</t>
+  </si>
+  <si>
+    <t>wage_exp=</t>
   </si>
 </sst>
 </file>
@@ -372,8 +417,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="271">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,12 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -692,11 +735,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="271">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -832,6 +881,8 @@
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -967,6 +1018,8 @@
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1298,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1310,7 +1363,7 @@
     <col min="5" max="29" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:21">
       <c r="A1" s="32" t="s">
         <v>32</v>
       </c>
@@ -1318,58 +1371,64 @@
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
     </row>
-    <row r="2" spans="1:17" ht="16" thickBot="1">
+    <row r="2" spans="1:21" ht="16" thickBot="1">
       <c r="A2" s="32"/>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
     </row>
-    <row r="3" spans="1:17">
-      <c r="D3" s="27" t="s">
+    <row r="3" spans="1:21">
+      <c r="D3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="28">
         <v>0</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="24">
         <v>0.25</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="24">
         <v>0.5</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="24">
         <v>0.75</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="24">
         <v>1</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="24">
         <v>1.25</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="24">
         <v>1.5</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="24">
         <v>1.75</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="24">
         <v>2</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="24">
         <v>2.25</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="24">
         <v>2.5</v>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="24">
         <v>2.75</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="29">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="D4" s="28" t="s">
+      <c r="T3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="7">
@@ -1411,9 +1470,15 @@
       <c r="Q4" s="11">
         <v>0.817339612770691</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="D5" s="28" t="s">
+      <c r="T4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="D5" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="7">
@@ -1455,9 +1520,15 @@
       <c r="Q5" s="11">
         <v>3.34935634376387</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="D6" s="28" t="s">
+      <c r="T5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="D6" s="26" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="8">
@@ -1499,9 +1570,15 @@
       <c r="Q6" s="12">
         <v>2.1412696232917999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="D7" s="28" t="s">
+      <c r="T6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1.7289771810981999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="D7" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="8">
@@ -1543,9 +1620,15 @@
       <c r="Q7" s="12">
         <v>1.99995251685427</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="D8" s="28" t="s">
+      <c r="T7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>1.8216685186138399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="D8" s="26" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="8">
@@ -1587,9 +1670,15 @@
       <c r="Q8" s="12">
         <v>2.0283070216816799</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="D9" s="28" t="s">
+      <c r="T8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1.9053375856233301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="D9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="8">
@@ -1631,9 +1720,15 @@
       <c r="Q9" s="12">
         <v>3.6008214909254201</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="D10" s="28" t="s">
+      <c r="T9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <v>3.67175082685378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="D10" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="8">
@@ -1675,9 +1770,15 @@
       <c r="Q10" s="12">
         <v>3.6221632131558601</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="D11" s="28" t="s">
+      <c r="T10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10">
+        <v>3.7080971704405301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="D11" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="8">
@@ -1719,9 +1820,15 @@
       <c r="Q11" s="12">
         <v>4.3571005725685001</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="D12" s="28" t="s">
+      <c r="T11" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11">
+        <v>5.8586996427434501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="D12" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="8">
@@ -1763,9 +1870,15 @@
       <c r="Q12" s="12">
         <v>3.1976937799979299</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="D13" s="28" t="s">
+      <c r="T12" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12">
+        <v>3.2481038760918901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="D13" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="8">
@@ -1807,9 +1920,15 @@
       <c r="Q13" s="12">
         <v>0.24218409457651699</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="D14" s="28" t="s">
+      <c r="T13" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13">
+        <v>0.380434438196316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="D14" s="26" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="8">
@@ -1851,9 +1970,15 @@
       <c r="Q14" s="12">
         <v>0.56650749185430604</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="D15" s="28" t="s">
+      <c r="T14" t="s">
+        <v>40</v>
+      </c>
+      <c r="U14">
+        <v>0.751789448655517</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="D15" s="26" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="8">
@@ -1895,9 +2020,15 @@
       <c r="Q15" s="12">
         <v>0.83720349380116998</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="D16" s="28" t="s">
+      <c r="T15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U15">
+        <v>0.80468455110585002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="D16" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="8">
@@ -1939,10 +2070,16 @@
       <c r="Q16" s="12">
         <v>0.38663436468772799</v>
       </c>
+      <c r="T16" t="s">
+        <v>21</v>
+      </c>
+      <c r="U16">
+        <v>0.33356444865960599</v>
+      </c>
     </row>
     <row r="17" spans="2:30">
       <c r="C17" s="1"/>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="8">
@@ -1983,13 +2120,19 @@
       </c>
       <c r="Q17" s="12">
         <v>7.08036220559429E-2</v>
+      </c>
+      <c r="T17" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" s="5">
+        <v>6.9372462643969804E-2</v>
       </c>
     </row>
     <row r="18" spans="2:30" ht="16" thickBot="1">
       <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="26" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="13">
@@ -2030,6 +2173,12 @@
       </c>
       <c r="Q18" s="14">
         <v>0.332094255492146</v>
+      </c>
+      <c r="T18" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18">
+        <v>0.999999999999998</v>
       </c>
     </row>
     <row r="19" spans="2:30">
@@ -2039,7 +2188,7 @@
       <c r="C19" s="15">
         <v>0.25422061206441499</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="25" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="17">
@@ -2089,7 +2238,7 @@
       <c r="C20" s="3">
         <v>6.0963892058338303</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="8">
@@ -2130,6 +2279,18 @@
       </c>
       <c r="Q20" s="12">
         <v>6.9473262844066896</v>
+      </c>
+      <c r="T20" t="s">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>0.28118921465207503</v>
+      </c>
+      <c r="V20" t="s">
+        <v>41</v>
+      </c>
+      <c r="W20">
+        <v>0.280933180577776</v>
       </c>
     </row>
     <row r="21" spans="2:30">
@@ -2139,7 +2300,7 @@
       <c r="C21" s="3">
         <v>0.54753382139812301</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="26" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="8">
@@ -2180,6 +2341,18 @@
       </c>
       <c r="Q21" s="12">
         <v>0.54715037129472899</v>
+      </c>
+      <c r="T21" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21">
+        <v>9.0876599951105401</v>
+      </c>
+      <c r="V21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W21">
+        <v>10.505562491752199</v>
       </c>
     </row>
     <row r="22" spans="2:30">
@@ -2189,7 +2362,7 @@
       <c r="C22" s="1">
         <v>1.21285622984174</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="8">
@@ -2230,6 +2403,18 @@
       </c>
       <c r="Q22" s="12">
         <v>1.26570159557661</v>
+      </c>
+      <c r="T22" t="s">
+        <v>8</v>
+      </c>
+      <c r="U22">
+        <v>0.46553818949426801</v>
+      </c>
+      <c r="V22" t="s">
+        <v>43</v>
+      </c>
+      <c r="W22">
+        <v>0.47189666007710401</v>
       </c>
     </row>
     <row r="23" spans="2:30">
@@ -2239,7 +2424,7 @@
       <c r="C23" s="1">
         <v>1.11645211458795</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="8">
@@ -2280,6 +2465,18 @@
       </c>
       <c r="Q23" s="12">
         <v>1.1650970560651199</v>
+      </c>
+      <c r="T23" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23">
+        <v>1.2411356290016</v>
+      </c>
+      <c r="V23" t="s">
+        <v>44</v>
+      </c>
+      <c r="W23">
+        <v>1.31385003766387</v>
       </c>
     </row>
     <row r="24" spans="2:30">
@@ -2289,7 +2486,7 @@
       <c r="C24" s="1">
         <v>7.8660707136206195E-2</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="8">
@@ -2330,6 +2527,18 @@
       </c>
       <c r="Q24" s="12">
         <v>7.2980921191854994E-2</v>
+      </c>
+      <c r="T24" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24">
+        <v>1.1424837201603699</v>
+      </c>
+      <c r="V24" t="s">
+        <v>45</v>
+      </c>
+      <c r="W24">
+        <v>1.2094184097918099</v>
       </c>
     </row>
     <row r="25" spans="2:30" ht="16" thickBot="1">
@@ -2339,7 +2548,7 @@
       <c r="C25" s="20">
         <v>1.4841342073060699</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="27" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="13">
@@ -2380,6 +2589,32 @@
       </c>
       <c r="Q25" s="14">
         <v>1.54988484615234</v>
+      </c>
+      <c r="T25" t="s">
+        <v>11</v>
+      </c>
+      <c r="U25" s="5">
+        <v>5.6198706516212199E-2</v>
+      </c>
+      <c r="V25" t="s">
+        <v>46</v>
+      </c>
+      <c r="W25" s="5">
+        <v>5.2213446171707499E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30">
+      <c r="T26" t="s">
+        <v>12</v>
+      </c>
+      <c r="U26">
+        <v>1.7862355660540501</v>
+      </c>
+      <c r="V26" t="s">
+        <v>47</v>
+      </c>
+      <c r="W26">
+        <v>1.8654074073992499</v>
       </c>
     </row>
     <row r="30" spans="2:30" ht="16" thickBot="1"/>
@@ -2467,80 +2702,80 @@
       <c r="D32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="30">
         <v>0</v>
       </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="22">
+      <c r="F32" s="31"/>
+      <c r="G32" s="30">
         <v>0.25</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="31">
         <v>0.25</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="30">
         <v>0.5</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="31">
         <v>0.5</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="30">
         <v>0.75</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="31">
         <v>0.75</v>
       </c>
-      <c r="M32" s="22">
+      <c r="M32" s="30">
         <v>1</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N32" s="31">
         <v>1</v>
       </c>
-      <c r="O32" s="25">
+      <c r="O32" s="23">
         <v>1.25</v>
       </c>
-      <c r="P32" s="24">
+      <c r="P32" s="22">
         <v>1.25</v>
       </c>
-      <c r="Q32" s="22">
+      <c r="Q32" s="30">
         <v>1.5</v>
       </c>
-      <c r="R32" s="23">
+      <c r="R32" s="31">
         <v>1.5</v>
       </c>
-      <c r="S32" s="22">
+      <c r="S32" s="30">
         <v>1.75</v>
       </c>
-      <c r="T32" s="23">
+      <c r="T32" s="31">
         <v>1.75</v>
       </c>
-      <c r="U32" s="22">
+      <c r="U32" s="30">
         <v>2</v>
       </c>
-      <c r="V32" s="23">
+      <c r="V32" s="31">
         <v>2</v>
       </c>
-      <c r="W32" s="22">
+      <c r="W32" s="30">
         <v>2.25</v>
       </c>
-      <c r="X32" s="23">
+      <c r="X32" s="31">
         <v>2.25</v>
       </c>
-      <c r="Y32" s="22">
+      <c r="Y32" s="30">
         <v>2.5</v>
       </c>
-      <c r="Z32" s="23">
+      <c r="Z32" s="31">
         <v>2.5</v>
       </c>
-      <c r="AA32" s="22">
+      <c r="AA32" s="30">
         <v>2.7</v>
       </c>
-      <c r="AB32" s="23">
+      <c r="AB32" s="31">
         <v>2.75</v>
       </c>
-      <c r="AC32" s="22">
+      <c r="AC32" s="30">
         <v>3</v>
       </c>
-      <c r="AD32" s="23">
+      <c r="AD32" s="31">
         <v>3</v>
       </c>
     </row>
@@ -4491,51 +4726,51 @@
   <sheetData>
     <row r="1" spans="2:16" ht="16" thickBot="1"/>
     <row r="2" spans="2:16">
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="28">
         <v>0</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="24">
         <v>0.25</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="24">
         <v>0.5</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="24">
         <v>0.75</v>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="24">
         <v>1</v>
       </c>
-      <c r="I2" s="26">
+      <c r="I2" s="24">
         <v>1.25</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="24">
         <v>1.5</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="24">
         <v>1.75</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="24">
         <v>2</v>
       </c>
-      <c r="M2" s="26">
+      <c r="M2" s="24">
         <v>2.25</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="24">
         <v>2.5</v>
       </c>
-      <c r="O2" s="26">
+      <c r="O2" s="24">
         <v>2.75</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:16">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="7">
@@ -4579,7 +4814,7 @@
       </c>
     </row>
     <row r="4" spans="2:16">
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="7">
@@ -4623,7 +4858,7 @@
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="8">
@@ -4667,7 +4902,7 @@
       </c>
     </row>
     <row r="6" spans="2:16">
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="8">
@@ -4711,7 +4946,7 @@
       </c>
     </row>
     <row r="7" spans="2:16">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="8">
@@ -4755,7 +4990,7 @@
       </c>
     </row>
     <row r="8" spans="2:16">
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="8">
@@ -4799,7 +5034,7 @@
       </c>
     </row>
     <row r="9" spans="2:16">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="8">
@@ -4843,7 +5078,7 @@
       </c>
     </row>
     <row r="10" spans="2:16">
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="8">
@@ -4887,7 +5122,7 @@
       </c>
     </row>
     <row r="11" spans="2:16">
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="8">
@@ -4931,7 +5166,7 @@
       </c>
     </row>
     <row r="12" spans="2:16">
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="8">
@@ -4975,7 +5210,7 @@
       </c>
     </row>
     <row r="13" spans="2:16">
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8">
@@ -5019,7 +5254,7 @@
       </c>
     </row>
     <row r="14" spans="2:16">
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="8">
@@ -5063,7 +5298,7 @@
       </c>
     </row>
     <row r="15" spans="2:16">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="8">
@@ -5108,7 +5343,7 @@
     </row>
     <row r="16" spans="2:16">
       <c r="B16" s="1"/>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="8">
@@ -5155,7 +5390,7 @@
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="13">
@@ -5205,7 +5440,7 @@
       <c r="B18" s="15">
         <v>0.25422061206441499</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="17">
@@ -5255,7 +5490,7 @@
       <c r="B19" s="3">
         <v>6.0963892058338303</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="8">
@@ -5305,7 +5540,7 @@
       <c r="B20" s="3">
         <v>0.54753382139812301</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="8">
@@ -5355,7 +5590,7 @@
       <c r="B21" s="1">
         <v>1.21285622984174</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="8">
@@ -5405,7 +5640,7 @@
       <c r="B22" s="1">
         <v>1.11645211458795</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="8">
@@ -5455,7 +5690,7 @@
       <c r="B23" s="1">
         <v>7.8660707136206195E-2</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="8">
@@ -5505,7 +5740,7 @@
       <c r="B24" s="20">
         <v>1.4841342073060699</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="13">

</xml_diff>